<commit_message>
ALL OUTJOBS, make all deliverables, eurocircuits visulizer PASS and quotation
</commit_message>
<xml_diff>
--- a/asm/Pick_Place.xlsx
+++ b/asm/Pick_Place.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20700" windowHeight="10155"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="10020"/>
   </bookViews>
   <sheets>
     <sheet name="Pick_Place" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
     <t>C6</t>
   </si>
   <si>
-    <t>30pF</t>
+    <t>33pF</t>
   </si>
   <si>
     <t>C7</t>
@@ -174,6 +174,9 @@
     <t>R8</t>
   </si>
   <si>
+    <t>R9</t>
+  </si>
+  <si>
     <t>R10</t>
   </si>
   <si>
@@ -186,9 +189,6 @@
     <t>0R</t>
   </si>
   <si>
-    <t>R13</t>
-  </si>
-  <si>
     <t>R14</t>
   </si>
   <si>
@@ -222,7 +222,7 @@
     <t>U2</t>
   </si>
   <si>
-    <t>NCP702N</t>
+    <t>TPS78233</t>
   </si>
   <si>
     <t>SOT23-5_0.95mm-NOSILK</t>
@@ -874,7 +874,7 @@
         <v>51</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>40</v>
@@ -882,10 +882,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>40</v>
@@ -893,10 +893,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Eurocircuits assembly output jobs
</commit_message>
<xml_diff>
--- a/asm/Pick_Place.xlsx
+++ b/asm/Pick_Place.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="10020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="8220"/>
   </bookViews>
   <sheets>
     <sheet name="Pick_Place" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="70">
   <si>
     <t>Designator</t>
   </si>
@@ -28,12 +28,6 @@
   </si>
   <si>
     <t>Footprint</t>
-  </si>
-  <si>
-    <t>B1</t>
-  </si>
-  <si>
-    <t>N-DAP</t>
   </si>
   <si>
     <t>C1</t>
@@ -583,7 +577,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -613,18 +607,18 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -632,43 +626,43 @@
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -676,120 +670,120 @@
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -797,32 +791,32 @@
         <v>41</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="C21" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -833,7 +827,7 @@
         <v>46</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -841,43 +835,43 @@
         <v>47</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="C26" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -888,7 +882,7 @@
         <v>53</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -896,21 +890,21 @@
         <v>54</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="C29" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -921,62 +915,51 @@
         <v>58</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="C32" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>